<commit_message>
started lab 2_2_3 report, updated some 2_1_2 stuff
</commit_message>
<xml_diff>
--- a/2_semester/labs/lab_2_1_2/Book2.xlsx
+++ b/2_semester/labs/lab_2_1_2/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\mipt_dgap\2_semester\labs\lab_2_1_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEB2900-1F08-456D-BD8E-9263B84D38B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206FEBB5-1FD9-4B1A-8FEF-03B688B95AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F71B547-3819-46F8-B34E-C27D7E74163A}"/>
+    <workbookView xWindow="29580" yWindow="675" windowWidth="21600" windowHeight="11385" xr2:uid="{9F71B547-3819-46F8-B34E-C27D7E74163A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -162,6 +162,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE74B5AD-BBF4-4C53-963D-9838BBD8F007}">
-  <dimension ref="C4:M92"/>
+  <dimension ref="C4:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,14 +501,16 @@
     <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85546875" style="1"/>
     <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="11" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="1"/>
-    <col min="13" max="13" width="35.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="8.85546875" style="1"/>
+    <col min="8" max="10" width="37.28515625" style="1" customWidth="1"/>
+    <col min="11" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="35.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,23 +526,23 @@
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" ht="60" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>20.6</v>
       </c>
@@ -548,22 +556,30 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="H5" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F5:G12)</f>
+        <v>10.6,0,10.4,20,10.3,40,10.2,55,10.1,70,10,100,10,120,9.9,160</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G5:G12)</f>
+        <v>0,20,40,55,70,100,120,160</v>
+      </c>
+      <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="L5" s="1">
         <v>9.9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <f>16.2-14.4</f>
         <v>1.7999999999999989</v>
       </c>
-      <c r="L5" s="1">
-        <f>J5/(J5-K5)</f>
+      <c r="N5" s="1">
+        <f>L5/(L5-M5)</f>
         <v>1.2222222222222221</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>20.5</v>
       </c>
@@ -577,25 +593,25 @@
       <c r="G6" s="1">
         <v>20</v>
       </c>
-      <c r="I6" s="1">
+      <c r="K6" s="1">
         <v>2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="L6" s="1">
         <v>9.1</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <f>16.1-14.3</f>
         <v>1.8000000000000007</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" ref="L6:L15" si="1">J6/(J6-K6)</f>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N15" si="1">L6/(L6-M6)</f>
         <v>1.2465753424657535</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <v>20.5</v>
       </c>
@@ -609,25 +625,25 @@
       <c r="G7" s="1">
         <v>40</v>
       </c>
-      <c r="I7" s="1">
+      <c r="K7" s="1">
         <v>3</v>
       </c>
-      <c r="J7" s="1">
+      <c r="L7" s="1">
         <v>9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <f>16.2-14.35</f>
         <v>1.8499999999999996</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <f t="shared" si="1"/>
         <v>1.2587412587412588</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -641,22 +657,22 @@
       <c r="G8" s="1">
         <v>55</v>
       </c>
-      <c r="I8" s="1">
+      <c r="K8" s="1">
         <v>4</v>
       </c>
-      <c r="J8" s="1">
+      <c r="L8" s="1">
         <v>9.3000000000000007</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <f>16.2-14.3</f>
         <v>1.8999999999999986</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <f t="shared" si="1"/>
         <v>1.2567567567567566</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -670,22 +686,22 @@
       <c r="G9" s="1">
         <v>70</v>
       </c>
-      <c r="J9" s="3">
+      <c r="L9" s="3">
         <v>9.4</v>
       </c>
-      <c r="K9" s="3">
+      <c r="M9" s="3">
         <f>16.6-14</f>
         <v>2.6000000000000014</v>
       </c>
-      <c r="L9" s="3">
+      <c r="N9" s="3">
         <f t="shared" si="1"/>
         <v>1.3823529411764708</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>20.3</v>
       </c>
@@ -699,25 +715,25 @@
       <c r="G10" s="1">
         <v>100</v>
       </c>
-      <c r="I10" s="1">
+      <c r="K10" s="1">
         <v>5</v>
       </c>
-      <c r="J10" s="1">
+      <c r="L10" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
         <f>16.5-14</f>
         <v>2.5</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1">
         <f t="shared" si="1"/>
         <v>1.3424657534246576</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>20.3</v>
       </c>
@@ -731,22 +747,22 @@
       <c r="G11" s="1">
         <v>120</v>
       </c>
-      <c r="I11" s="1">
+      <c r="K11" s="1">
         <v>6</v>
       </c>
-      <c r="J11" s="1">
+      <c r="L11" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K11" s="1">
+      <c r="M11" s="1">
         <f>16.4-14.1</f>
         <v>2.2999999999999989</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1">
         <f t="shared" si="1"/>
         <v>1.3066666666666664</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>20.3</v>
       </c>
@@ -760,22 +776,24 @@
       <c r="G12" s="2">
         <v>160</v>
       </c>
-      <c r="I12" s="1">
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="K12" s="1">
         <v>7</v>
       </c>
-      <c r="J12" s="1">
+      <c r="L12" s="1">
         <v>9.5</v>
       </c>
-      <c r="K12" s="1">
+      <c r="M12" s="1">
         <f>16.4-14.2</f>
         <v>2.1999999999999993</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <f t="shared" si="1"/>
         <v>1.3013698630136985</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" ht="60" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>20.5</v>
       </c>
@@ -783,28 +801,36 @@
         <v>10</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="0"/>
+        <f>D13-E13</f>
         <v>10.5</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="H13" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F13:F20)</f>
+        <v>10.5,10.1,9.6,9.4,9.3,9.2,9.2,9.1</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G13:G20)</f>
+        <v>0,20,45,75,90,105,140,170</v>
+      </c>
+      <c r="K13" s="1">
         <v>8</v>
       </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1">
         <v>9.4</v>
       </c>
-      <c r="K13" s="1">
+      <c r="M13" s="1">
         <f>16.3-14.2</f>
         <v>2.1000000000000014</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1">
         <f t="shared" si="1"/>
         <v>1.2876712328767126</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -818,22 +844,22 @@
       <c r="G14" s="1">
         <v>20</v>
       </c>
-      <c r="I14" s="1">
+      <c r="K14" s="1">
         <v>9</v>
       </c>
-      <c r="J14" s="1">
+      <c r="L14" s="1">
         <v>9.6</v>
       </c>
-      <c r="K14" s="1">
+      <c r="M14" s="1">
         <f>16.4-14.2</f>
         <v>2.1999999999999993</v>
       </c>
-      <c r="L14" s="1">
+      <c r="N14" s="1">
         <f t="shared" si="1"/>
         <v>1.2972972972972971</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -847,22 +873,22 @@
       <c r="G15" s="1">
         <v>45</v>
       </c>
-      <c r="I15" s="1">
+      <c r="K15" s="1">
         <v>10</v>
       </c>
-      <c r="J15" s="1">
+      <c r="L15" s="1">
         <v>9.5</v>
       </c>
-      <c r="K15" s="1">
+      <c r="M15" s="1">
         <f>16.4-14.2</f>
         <v>2.1999999999999993</v>
       </c>
-      <c r="L15" s="1">
+      <c r="N15" s="1">
         <f t="shared" si="1"/>
         <v>1.3013698630136985</v>
       </c>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>20</v>
       </c>
@@ -877,7 +903,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>20</v>
       </c>
@@ -892,7 +918,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>19.899999999999999</v>
       </c>
@@ -907,7 +933,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>19.899999999999999</v>
       </c>
@@ -921,17 +947,17 @@
       <c r="G19" s="1">
         <v>140</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <v>19.899999999999999</v>
       </c>
@@ -945,19 +971,21 @@
       <c r="G20" s="2">
         <v>170</v>
       </c>
-      <c r="K20" s="1">
-        <f>AVERAGE(L20:L30)</f>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="M20" s="1">
+        <f>AVERAGE(N20:N30)</f>
         <v>1.2821136256478722</v>
       </c>
-      <c r="L20" s="1">
+      <c r="N20" s="1">
         <v>1.2222222222222221</v>
       </c>
-      <c r="M20" s="1">
-        <f>(L20-$K$20)^2</f>
+      <c r="O20" s="1">
+        <f>(N20-$M$20)^2</f>
         <v>3.5869802042939767E-3</v>
       </c>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:15" ht="75" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>20.5</v>
       </c>
@@ -971,15 +999,23 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="L21" s="1">
+      <c r="H21" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F21:F30)</f>
+        <v>10.6,10.1,9.8,9.6,9.5,9.4,9.3,9.3,9.2,9</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G21:G30)</f>
+        <v>0,30,50,70,100,120,150,180,210,250</v>
+      </c>
+      <c r="N21" s="1">
         <v>1.2465753424657535</v>
       </c>
-      <c r="M21" s="1">
-        <f t="shared" ref="M21:M29" si="2">(L21-$K$20)^2</f>
+      <c r="O21" s="1">
+        <f t="shared" ref="O21:O29" si="2">(N21-$M$20)^2</f>
         <v>1.2629695715324618E-3</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -993,15 +1029,15 @@
       <c r="G22" s="1">
         <v>30</v>
       </c>
-      <c r="L22" s="1">
+      <c r="N22" s="1">
         <v>1.2587412587412588</v>
       </c>
-      <c r="M22" s="1">
+      <c r="O22" s="1">
         <f t="shared" si="2"/>
         <v>5.4626753481736121E-4</v>
       </c>
     </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>20.2</v>
       </c>
@@ -1015,15 +1051,15 @@
       <c r="G23" s="1">
         <v>50</v>
       </c>
-      <c r="L23" s="1">
+      <c r="N23" s="1">
         <v>1.2567567567567566</v>
       </c>
-      <c r="M23" s="1">
+      <c r="O23" s="1">
         <f t="shared" si="2"/>
         <v>6.4297079996122907E-4</v>
       </c>
     </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1037,15 +1073,15 @@
       <c r="G24" s="1">
         <v>70</v>
       </c>
-      <c r="L24" s="1">
+      <c r="N24" s="1">
         <v>1.3424657534246576</v>
       </c>
-      <c r="M24" s="1">
+      <c r="O24" s="1">
         <f t="shared" si="2"/>
         <v>3.642379327185424E-3</v>
       </c>
     </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1059,15 +1095,15 @@
       <c r="G25" s="1">
         <v>100</v>
       </c>
-      <c r="L25" s="1">
+      <c r="N25" s="1">
         <v>1.3066666666666664</v>
       </c>
-      <c r="M25" s="1">
+      <c r="O25" s="1">
         <f t="shared" si="2"/>
         <v>6.0285182327058989E-4</v>
       </c>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>20</v>
       </c>
@@ -1081,15 +1117,15 @@
       <c r="G26" s="1">
         <v>120</v>
       </c>
-      <c r="L26" s="1">
+      <c r="N26" s="1">
         <v>1.3013698630136985</v>
       </c>
-      <c r="M26" s="1">
+      <c r="O26" s="1">
         <f t="shared" si="2"/>
         <v>3.7080267748904375E-4</v>
       </c>
     </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>20</v>
       </c>
@@ -1103,15 +1139,15 @@
       <c r="G27" s="1">
         <v>150</v>
       </c>
-      <c r="L27" s="1">
+      <c r="N27" s="1">
         <v>1.2876712328767126</v>
       </c>
-      <c r="M27" s="1">
+      <c r="O27" s="1">
         <f t="shared" si="2"/>
         <v>3.0886998110058574E-5</v>
       </c>
     </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>20</v>
       </c>
@@ -1125,15 +1161,15 @@
       <c r="G28" s="1">
         <v>180</v>
       </c>
-      <c r="L28" s="1">
+      <c r="N28" s="1">
         <v>1.2972972972972971</v>
       </c>
-      <c r="M28" s="1">
+      <c r="O28" s="1">
         <f t="shared" si="2"/>
         <v>2.3054388475754985E-4</v>
       </c>
     </row>
-    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>19.899999999999999</v>
       </c>
@@ -1147,15 +1183,15 @@
       <c r="G29" s="1">
         <v>210</v>
       </c>
-      <c r="L29" s="1">
+      <c r="N29" s="1">
         <v>1.3013698630136985</v>
       </c>
-      <c r="M29" s="1">
+      <c r="O29" s="1">
         <f t="shared" si="2"/>
         <v>3.7080267748904375E-4</v>
       </c>
     </row>
-    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <v>19.8</v>
       </c>
@@ -1169,15 +1205,17 @@
       <c r="G30" s="2">
         <v>250</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="N30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M30" s="1">
-        <f>SUM(M20:M29)</f>
+      <c r="O30" s="1">
+        <f>SUM(O20:O29)</f>
         <v>1.1287455498906739E-2</v>
       </c>
     </row>
-    <row r="31" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:15" ht="60" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>20.5</v>
       </c>
@@ -1191,15 +1229,23 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="H31" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F31:F38)</f>
+        <v>10.5,10,9.8,9.8,9.6,9.4,9.3,9.3</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G31:G38)</f>
+        <v>0,40,60,80,120,180,240,300</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M31" s="1">
-        <f>SQRT(M30/10)</f>
+      <c r="O31" s="1">
+        <f>SQRT(O30/10)</f>
         <v>3.3596808626574548E-2</v>
       </c>
     </row>
-    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>20.3</v>
       </c>
@@ -1214,7 +1260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <v>20.2</v>
       </c>
@@ -1228,15 +1274,15 @@
       <c r="G33" s="1">
         <v>60</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M33" s="1">
-        <f>K20*SQRT((0.05)^2+(0.1/10)^2+(0.1/2.5)^2)</f>
+      <c r="O33" s="1">
+        <f>M20*SQRT((0.05)^2+(0.1/10)^2+(0.1/2.5)^2)</f>
         <v>8.3090459537194267E-2</v>
       </c>
     </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>20.2</v>
       </c>
@@ -1251,7 +1297,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="4:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1265,15 +1311,15 @@
       <c r="G35" s="1">
         <v>120</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M35" s="1">
-        <f>SQRT(M31^2+M33^2)</f>
+      <c r="O35" s="1">
+        <f>SQRT(O31^2+O33^2)</f>
         <v>8.9625721843635889E-2</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>20</v>
       </c>
@@ -1287,12 +1333,12 @@
       <c r="G36" s="1">
         <v>180</v>
       </c>
-      <c r="M36" s="1">
-        <f>M35/K20</f>
+      <c r="O36" s="1">
+        <f>O35/M20</f>
         <v>6.990466371367561E-2</v>
       </c>
     </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>19.899999999999999</v>
       </c>
@@ -1307,7 +1353,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <v>19.899999999999999</v>
       </c>
@@ -1321,8 +1367,10 @@
       <c r="G38" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D39" s="3">
         <v>20.5</v>
       </c>
@@ -1336,8 +1384,10 @@
       <c r="G39" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D40" s="3">
         <v>20.2</v>
       </c>
@@ -1351,8 +1401,10 @@
       <c r="G40" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D41" s="3">
         <v>20.100000000000001</v>
       </c>
@@ -1366,8 +1418,10 @@
       <c r="G41" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D42" s="3">
         <v>20.100000000000001</v>
       </c>
@@ -1381,8 +1435,10 @@
       <c r="G42" s="3">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D43" s="3">
         <v>20</v>
       </c>
@@ -1396,8 +1452,10 @@
       <c r="G43" s="3">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D44" s="3">
         <v>20</v>
       </c>
@@ -1411,8 +1469,10 @@
       <c r="G44" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D45" s="3">
         <v>20</v>
       </c>
@@ -1426,8 +1486,10 @@
       <c r="G45" s="3">
         <v>180</v>
       </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D46" s="4">
         <v>20</v>
       </c>
@@ -1441,8 +1503,10 @@
       <c r="G46" s="4">
         <v>240</v>
       </c>
-    </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="4:15" ht="60" x14ac:dyDescent="0.25">
       <c r="D47" s="1">
         <v>20.5</v>
       </c>
@@ -1456,8 +1520,16 @@
       <c r="G47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F47:F55)</f>
+        <v>10.6,10.2,10,9.8,9.8,9.8,9.8,9.8,9.9</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G47:G55)</f>
+        <v>0,20,45,70,100,120,150,180,240</v>
+      </c>
+    </row>
+    <row r="48" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D48" s="1">
         <v>20.399999999999999</v>
       </c>
@@ -1472,7 +1544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D49" s="1">
         <v>20.3</v>
       </c>
@@ -1487,7 +1559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D50" s="1">
         <v>20.2</v>
       </c>
@@ -1502,7 +1574,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D51" s="1">
         <v>20.2</v>
       </c>
@@ -1517,7 +1589,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D52" s="1">
         <v>20.2</v>
       </c>
@@ -1532,7 +1604,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D53" s="1">
         <v>20.2</v>
       </c>
@@ -1547,7 +1619,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D54" s="1">
         <v>20.2</v>
       </c>
@@ -1562,7 +1634,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
         <v>20.2</v>
       </c>
@@ -1576,8 +1648,10 @@
       <c r="G55" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D56" s="1">
         <v>20.5</v>
       </c>
@@ -1591,8 +1665,16 @@
       <c r="G56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F56:F62)</f>
+        <v>10.5,10,9.8,9.8,9.8,9.8,9.8</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G56:G62)</f>
+        <v>0,30,60,90,120,180,240</v>
+      </c>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D57" s="1">
         <v>20.3</v>
       </c>
@@ -1607,7 +1689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D58" s="1">
         <v>20.2</v>
       </c>
@@ -1622,7 +1704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D59" s="1">
         <v>20.2</v>
       </c>
@@ -1637,7 +1719,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D60" s="1">
         <v>20.2</v>
       </c>
@@ -1652,7 +1734,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D61" s="1">
         <v>20.2</v>
       </c>
@@ -1667,7 +1749,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D62" s="2">
         <v>20.2</v>
       </c>
@@ -1681,8 +1763,10 @@
       <c r="G62" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D63" s="1">
         <v>20.5</v>
       </c>
@@ -1696,8 +1780,16 @@
       <c r="G63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F63:F69)</f>
+        <v>10.5,9.9,9.6,9.5,9.5,9.5,9.5</v>
+      </c>
+      <c r="I63" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G63:G69)</f>
+        <v>0,30,60,90,120,180,240</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D64" s="1">
         <v>20.3</v>
       </c>
@@ -1712,7 +1804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D65" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1727,7 +1819,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D66" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1742,7 +1834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D67" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1757,7 +1849,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D68" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1772,7 +1864,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D69" s="2">
         <v>20.100000000000001</v>
       </c>
@@ -1786,8 +1878,10 @@
       <c r="G69" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D70" s="1">
         <v>20.5</v>
       </c>
@@ -1801,8 +1895,16 @@
       <c r="G70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F70:F76)</f>
+        <v>10.5,9.8,9.6,9.6,9.5,9.4,9.4</v>
+      </c>
+      <c r="I70" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G70:G76)</f>
+        <v>0,30,60,90,120,180,240</v>
+      </c>
+    </row>
+    <row r="71" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D71" s="1">
         <v>20.2</v>
       </c>
@@ -1817,7 +1919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D72" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1832,7 +1934,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D73" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1847,7 +1949,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D74" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1862,7 +1964,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D75" s="1">
         <v>20</v>
       </c>
@@ -1877,7 +1979,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D76" s="2">
         <v>20</v>
       </c>
@@ -1891,8 +1993,10 @@
       <c r="G76" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+    </row>
+    <row r="77" spans="4:9" ht="45" x14ac:dyDescent="0.25">
       <c r="D77" s="1">
         <v>20.5</v>
       </c>
@@ -1906,8 +2010,16 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F77:F83)</f>
+        <v>10.5,9.9,9.8,9.7,9.7,9.6,9.6</v>
+      </c>
+      <c r="I77" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G77:G83)</f>
+        <v>0,30,60,90,120,180,240</v>
+      </c>
+    </row>
+    <row r="78" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D78" s="1">
         <v>20.3</v>
       </c>
@@ -1922,7 +2034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D79" s="1">
         <v>20.2</v>
       </c>
@@ -1937,7 +2049,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D80" s="1">
         <v>20.2</v>
       </c>
@@ -1952,7 +2064,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D81" s="1">
         <v>20.2</v>
       </c>
@@ -1967,7 +2079,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D82" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -1982,7 +2094,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D83" s="2">
         <v>20.100000000000001</v>
       </c>
@@ -1996,8 +2108,10 @@
       <c r="G83" s="2">
         <v>240</v>
       </c>
-    </row>
-    <row r="84" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+    </row>
+    <row r="84" spans="4:9" ht="60" x14ac:dyDescent="0.25">
       <c r="D84" s="1">
         <v>20.5</v>
       </c>
@@ -2011,8 +2125,16 @@
       <c r="G84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,F84:F91)</f>
+        <v>10.5,10,9.8,9.7,9.6,9.6,9.5,9.5</v>
+      </c>
+      <c r="I84" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,G84:G91)</f>
+        <v>0,20,40,60,90,120,180,240</v>
+      </c>
+    </row>
+    <row r="85" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D85" s="1">
         <v>20.3</v>
       </c>
@@ -2027,7 +2149,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D86" s="1">
         <v>20.2</v>
       </c>
@@ -2042,7 +2164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D87" s="1">
         <v>20.2</v>
       </c>
@@ -2057,7 +2179,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D88" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -2072,7 +2194,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D89" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -2087,7 +2209,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="90" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D90" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -2102,7 +2224,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D91" s="1">
         <v>20.100000000000001</v>
       </c>
@@ -2117,7 +2239,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:9" x14ac:dyDescent="0.25">
       <c r="F92" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>